<commit_message>
Fix: Corregida ruta del template login.html y reorganización de estructura de carpetas
</commit_message>
<xml_diff>
--- a/bd/registros.xlsx
+++ b/bd/registros.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,6 +1123,206 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Eliminó producto: Yuval (ID 3)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2026-02-16 17:02:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2026-02-16 17:16:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2026-02-16 22:34:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2026-02-16 23:25:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2026-02-17 00:32:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2026-02-17 00:42:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:03:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2026-02-17 13:34:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:37:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>nico@gmail.com</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Inicio de sesión exitoso</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2026-02-17 14:38:12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>